<commit_message>
2012-9-14 sashimi update the ip address.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST969_AddAndCopyView.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST969_AddAndCopyView.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="2535" windowWidth="18195" windowHeight="14070"/>
+    <workbookView xWindow="270" yWindow="2535" windowWidth="15480" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="3" r:id="rId1"/>
@@ -4849,7 +4849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>

</xml_diff>